<commit_message>
starting point for 2015 data
</commit_message>
<xml_diff>
--- a/gals15.xlsx
+++ b/gals15.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t xml:space="preserve">2015 data</t>
   </si>
@@ -124,6 +124,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -141,7 +142,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +153,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
     <fill>
@@ -195,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,6 +215,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -217,6 +232,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -225,13 +300,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M:M"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="28:28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.75"/>
@@ -254,44 +329,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -315,76 +391,76 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="4" t="n">
         <v>3608</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="4" t="n">
         <v>3654</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="4" t="n">
         <v>415</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="4" t="n">
         <v>250</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="I4" s="4" t="n">
         <v>16.69</v>
       </c>
-      <c r="J4" s="2" t="n">
+      <c r="J4" s="4" t="n">
         <v>0.13</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="4" t="n">
         <v>4.3</v>
       </c>
-      <c r="L4" s="2" t="n">
+      <c r="L4" s="4" t="n">
         <v>1.06</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="6" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="4" t="n">
         <v>3057.6</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="4" t="n">
         <v>3160.4</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="4" t="n">
         <v>342</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="4" t="n">
         <v>300</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="4" t="n">
         <v>1200</v>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="I6" s="4" t="n">
         <v>65.44</v>
       </c>
-      <c r="J6" s="2" t="n">
+      <c r="J6" s="4" t="n">
         <v>0.15</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="K6" s="4" t="n">
         <v>4.4</v>
       </c>
-      <c r="L6" s="2" t="n">
+      <c r="L6" s="4" t="n">
         <v>1.06</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -575,44 +651,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B29" s="0" t="n">
         <v>4652</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D29" s="0" t="n">
         <v>4669</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <v>385</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="G28" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H28" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I28" s="0" t="n">
-        <v>15.89</v>
-      </c>
-      <c r="J28" s="0" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="K28" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="L28" s="0" t="n">
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="0" t="n">
-        <v>4670</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>385</v>
@@ -621,59 +710,59 @@
         <v>250</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I29" s="0" t="n">
-        <v>16.82</v>
+        <v>15.89</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>0.22</v>
       </c>
       <c r="K29" s="0" t="n">
-        <v>5.2</v>
+        <v>5.1</v>
       </c>
       <c r="L29" s="0" t="n">
-        <v>1.07</v>
-      </c>
-      <c r="N29" s="0" t="s">
-        <v>28</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="0" t="n">
-        <v>4672</v>
+        <v>4670</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>374</v>
+        <v>385</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>250</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="I30" s="0" t="n">
-        <v>15.91</v>
+        <v>16.82</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>0.22</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>2.6</v>
+        <v>5.2</v>
       </c>
       <c r="L30" s="0" t="n">
-        <v>1.15</v>
+        <v>1.07</v>
+      </c>
+      <c r="N30" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="0" t="n">
-        <v>4673</v>
+        <v>4672</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>374</v>
@@ -682,24 +771,53 @@
         <v>250</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>12</v>
       </c>
       <c r="I31" s="0" t="n">
-        <v>16.86</v>
+        <v>15.91</v>
       </c>
       <c r="J31" s="0" t="n">
         <v>0.22</v>
       </c>
       <c r="K31" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>1.15</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="0" t="n">
+        <v>4673</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>374</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>16.86</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="K32" s="0" t="n">
         <v>2.5</v>
       </c>
-      <c r="L31" s="0" t="n">
+      <c r="L32" s="0" t="n">
         <v>1.33</v>
       </c>
-      <c r="N31" s="0" t="s">
+      <c r="N32" s="0" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>